<commit_message>
Needs adjustments before Coding/Testing exam
</commit_message>
<xml_diff>
--- a/Assets/Maps/map_2.xlsx
+++ b/Assets/Maps/map_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msals\Desktop\map\2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdulaziz\Documents\CPCS-499\Project\Trip-Navigator-2D\Assets\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67A22D9-996F-46C9-84FA-9E2073163026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959BDA13-891F-49AA-8752-9A060F101E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{571CE9F3-7F1B-4A25-A89A-3D67A6FFCAFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{571CE9F3-7F1B-4A25-A89A-3D67A6FFCAFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="2">
+  <si>
+    <t>4L</t>
+  </si>
+  <si>
+    <t>4R</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF29894A-F3B9-48B0-9162-1AB5F25AF7E7}">
   <dimension ref="A1:CJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AS19" sqref="AS19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="CK31" sqref="CK31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,257 +5268,257 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1">
-        <v>4</v>
-      </c>
-      <c r="H19" s="1">
-        <v>4</v>
-      </c>
-      <c r="I19" s="1">
-        <v>4</v>
-      </c>
-      <c r="J19" s="1">
-        <v>4</v>
-      </c>
-      <c r="K19" s="1">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1">
-        <v>4</v>
-      </c>
-      <c r="M19" s="1">
-        <v>4</v>
-      </c>
-      <c r="N19" s="1">
-        <v>4</v>
-      </c>
-      <c r="O19" s="1">
-        <v>4</v>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
       </c>
-      <c r="Q19" s="1">
-        <v>4</v>
-      </c>
-      <c r="R19" s="1">
-        <v>4</v>
-      </c>
-      <c r="S19" s="1">
-        <v>4</v>
-      </c>
-      <c r="T19" s="1">
-        <v>4</v>
+      <c r="Q19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U19" s="1">
         <v>1</v>
       </c>
-      <c r="V19" s="1">
-        <v>4</v>
-      </c>
-      <c r="W19" s="1">
-        <v>4</v>
-      </c>
-      <c r="X19" s="1">
-        <v>4</v>
-      </c>
-      <c r="Y19" s="1">
-        <v>4</v>
-      </c>
-      <c r="Z19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AB19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AC19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AD19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AE19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AF19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AG19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AH19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AI19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AJ19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AK19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AL19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AM19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AN19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AO19" s="1">
-        <v>4</v>
+      <c r="V19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="AP19" s="1">
         <v>1</v>
       </c>
-      <c r="AQ19" s="1">
-        <v>4</v>
+      <c r="AQ19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="AR19" s="1">
         <v>1</v>
       </c>
-      <c r="AS19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AT19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AU19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AV19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AW19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AX19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AY19" s="1">
-        <v>4</v>
-      </c>
-      <c r="AZ19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BA19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BB19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BC19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BD19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BE19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BF19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BG19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BH19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BI19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BJ19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BK19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BL19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BM19" s="1">
-        <v>4</v>
+      <c r="AS19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="BN19" s="1">
         <v>1</v>
       </c>
-      <c r="BO19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BP19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BQ19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BR19" s="1">
-        <v>4</v>
+      <c r="BO19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="BS19" s="1">
         <v>1</v>
       </c>
-      <c r="BT19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BU19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BV19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BW19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BX19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BY19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BZ19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CA19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CB19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CC19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CD19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CE19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CF19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CG19" s="1">
-        <v>4</v>
-      </c>
-      <c r="CH19" s="1">
-        <v>4</v>
+      <c r="BT19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BU19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BV19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BY19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BZ19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CB19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CC19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CD19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CF19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CG19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CH19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="CI19" s="1">
         <v>1</v>
@@ -5789,257 +5800,257 @@
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4</v>
-      </c>
-      <c r="G21" s="1">
-        <v>4</v>
-      </c>
-      <c r="H21" s="1">
-        <v>4</v>
-      </c>
-      <c r="I21" s="1">
-        <v>4</v>
-      </c>
-      <c r="J21" s="1">
-        <v>4</v>
-      </c>
-      <c r="K21" s="1">
-        <v>4</v>
-      </c>
-      <c r="L21" s="1">
-        <v>4</v>
-      </c>
-      <c r="M21" s="1">
-        <v>4</v>
-      </c>
-      <c r="N21" s="1">
-        <v>4</v>
-      </c>
-      <c r="O21" s="1">
-        <v>4</v>
-      </c>
-      <c r="P21" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>4</v>
-      </c>
-      <c r="R21" s="1">
-        <v>4</v>
-      </c>
-      <c r="S21" s="1">
-        <v>4</v>
-      </c>
-      <c r="T21" s="1">
-        <v>4</v>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="U21" s="1">
         <v>1</v>
       </c>
-      <c r="V21" s="1">
-        <v>4</v>
-      </c>
-      <c r="W21" s="1">
-        <v>4</v>
-      </c>
-      <c r="X21" s="1">
-        <v>4</v>
-      </c>
-      <c r="Y21" s="1">
-        <v>4</v>
+      <c r="V21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="Z21" s="1">
         <v>1</v>
       </c>
-      <c r="AA21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AB21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AC21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AD21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AE21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AF21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AG21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AH21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AI21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AJ21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AK21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AL21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AM21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AN21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AO21" s="1">
-        <v>4</v>
+      <c r="AA21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="AP21" s="1">
         <v>1</v>
       </c>
-      <c r="AQ21" s="1">
-        <v>4</v>
+      <c r="AQ21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="AR21" s="1">
         <v>1</v>
       </c>
-      <c r="AS21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AT21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AU21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AV21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AW21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AX21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AY21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AZ21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BA21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BB21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BC21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BD21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BE21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BF21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BG21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BH21" s="1">
-        <v>4</v>
+      <c r="AS21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="BI21" s="1">
         <v>1</v>
       </c>
-      <c r="BJ21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BK21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BL21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BM21" s="1">
-        <v>4</v>
+      <c r="BJ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BK21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BM21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="BN21" s="1">
         <v>1</v>
       </c>
-      <c r="BO21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BP21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BQ21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BR21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BS21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BT21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BU21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BV21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BW21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BX21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BY21" s="1">
-        <v>4</v>
-      </c>
-      <c r="BZ21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CA21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CB21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CC21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CD21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CE21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CF21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CG21" s="1">
-        <v>4</v>
-      </c>
-      <c r="CH21" s="1">
-        <v>4</v>
+      <c r="BO21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BP21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BR21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BU21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BY21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CA21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CB21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CC21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CD21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CE21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CF21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CG21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="CI21" s="1">
         <v>1</v>

</xml_diff>